<commit_message>
Cargado ejemplos corregido, más pequeños fix
</commit_message>
<xml_diff>
--- a/clcore/output/StructureDefinition-CodigoPaises.xlsx
+++ b/clcore/output/StructureDefinition-CodigoPaises.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AK$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AK$17</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="168">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.5</t>
+    <t>1.8.6</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-31T17:56:54-03:00</t>
+    <t>2023-11-09T12:29:21-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -136,6 +136,117 @@
   </si>
   <si>
     <t>element:Element</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Slice Name</t>
+  </si>
+  <si>
+    <t>Alias(s)</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Must Support?</t>
+  </si>
+  <si>
+    <t>Is Modifier?</t>
+  </si>
+  <si>
+    <t>Is Summary?</t>
+  </si>
+  <si>
+    <t>Type(s)</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>Meaning When Missing</t>
+  </si>
+  <si>
+    <t>Fixed Value</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Minimum Value</t>
+  </si>
+  <si>
+    <t>Maximum Value</t>
+  </si>
+  <si>
+    <t>Maximum Length</t>
+  </si>
+  <si>
+    <t>Binding Strength</t>
+  </si>
+  <si>
+    <t>Binding Description</t>
+  </si>
+  <si>
+    <t>Binding Value Set</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Slicing Discriminator</t>
+  </si>
+  <si>
+    <t>Slicing Description</t>
+  </si>
+  <si>
+    <t>Slicing Ordered</t>
+  </si>
+  <si>
+    <t>Slicing Rules</t>
+  </si>
+  <si>
+    <t>Base Path</t>
+  </si>
+  <si>
+    <t>Base Min</t>
+  </si>
+  <si>
+    <t>Base Max</t>
+  </si>
+  <si>
+    <t>Condition(s)</t>
+  </si>
+  <si>
+    <t>Constraint(s)</t>
+  </si>
+  <si>
+    <t>Mapping: RIM Mapping</t>
   </si>
   <si>
     <t/>
@@ -751,7 +862,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK16"/>
+  <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -760,1719 +871,1833 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="35.67578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="35.67578125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.203125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="6" max="6" width="2.203125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="2.203125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="2.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="35.94921875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="35.94921875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.6640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="16.8359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="221.62109375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="221.59375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="8.5625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="46.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="9.2890625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0859375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="5.484375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="23.2734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="2.203125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="2.203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" hidden="true" width="8.0" customWidth="false"/>
-    <col min="17" max="17" width="20.703125" customWidth="true"/>
+    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="18.9140625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="46.1484375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="23.3359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="45.9453125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="45.8671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" t="s" s="2">
+      <c r="A1" t="s" s="1">
         <v>40</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" t="s" s="2">
+      <c r="B1" t="s" s="1">
         <v>41</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="C1" t="s" s="1">
         <v>42</v>
       </c>
-      <c r="H1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="K1" t="s" s="2">
+      <c r="D1" t="s" s="1">
         <v>43</v>
       </c>
-      <c r="L1" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AF1" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH1" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI1" t="s" s="2">
+      <c r="E1" t="s" s="1">
         <v>44</v>
       </c>
-      <c r="AJ1" t="s" s="2">
+      <c r="F1" t="s" s="1">
         <v>45</v>
       </c>
-      <c r="AK1" t="s" s="2">
-        <v>40</v>
+      <c r="G1" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s" s="1">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s" s="1">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s" s="1">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s" s="1">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s" s="1">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s" s="1">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s" s="1">
+        <v>55</v>
+      </c>
+      <c r="Q1" t="s" s="1">
+        <v>56</v>
+      </c>
+      <c r="R1" t="s" s="1">
+        <v>57</v>
+      </c>
+      <c r="S1" t="s" s="1">
+        <v>58</v>
+      </c>
+      <c r="T1" t="s" s="1">
+        <v>59</v>
+      </c>
+      <c r="U1" t="s" s="1">
+        <v>60</v>
+      </c>
+      <c r="V1" t="s" s="1">
+        <v>61</v>
+      </c>
+      <c r="W1" t="s" s="1">
+        <v>62</v>
+      </c>
+      <c r="X1" t="s" s="1">
+        <v>63</v>
+      </c>
+      <c r="Y1" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="Z1" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="AA1" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="AB1" t="s" s="1">
+        <v>67</v>
+      </c>
+      <c r="AC1" t="s" s="1">
+        <v>68</v>
+      </c>
+      <c r="AD1" t="s" s="1">
+        <v>69</v>
+      </c>
+      <c r="AE1" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="AF1" t="s" s="1">
+        <v>71</v>
+      </c>
+      <c r="AG1" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="AH1" t="s" s="1">
+        <v>73</v>
+      </c>
+      <c r="AI1" t="s" s="1">
+        <v>74</v>
+      </c>
+      <c r="AJ1" t="s" s="1">
+        <v>75</v>
+      </c>
+      <c r="AK1" t="s" s="1">
+        <v>76</v>
       </c>
     </row>
     <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>52</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="AK3" t="s" s="2">
-        <v>40</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="N4" t="s" s="2">
-        <v>64</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="N5" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="N5" t="s" s="2">
+        <v>101</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" t="s" s="2">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>65</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="N7" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="AC7" t="s" s="2">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="AD7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="O8" t="s" s="2">
-        <v>83</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB8" t="s" s="2">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="AC8" t="s" s="2">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="AD8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH8" t="s" s="2">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="N9" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="O9" t="s" s="2">
+        <v>120</v>
+      </c>
       <c r="P9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="AG9" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH9" t="s" s="2">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>52</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="AG10" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="O11" t="s" s="2">
-        <v>92</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="O11" s="2"/>
       <c r="P11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB11" t="s" s="2">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="AC11" t="s" s="2">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="AD11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AG11" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="O12" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="O12" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="P12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AC12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AD12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>100</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="N13" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="Y13" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="Y13" t="s" s="2">
+        <v>77</v>
+      </c>
       <c r="Z13" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA13" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB13" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC13" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD13" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE13" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF13" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="AG13" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH13" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI13" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ13" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="AA13" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB13" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC13" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD13" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE13" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AF13" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="AG13" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH13" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AI13" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ13" t="s" s="2">
-        <v>70</v>
-      </c>
       <c r="AK13" t="s" s="2">
-        <v>109</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>48</v>
+        <v>139</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="P14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y14" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="Y14" s="2"/>
       <c r="Z14" t="s" s="2">
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="AA14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AC14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AD14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>115</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>120</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
-        <v>121</v>
+        <v>150</v>
       </c>
       <c r="P15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AC15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>123</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="P16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="S16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="T16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="U16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="V16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AB16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AC16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>130</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" hidden="true">
+      <c r="A17" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G17" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J17" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L17" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="M17" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="N17" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="O17" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="P17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q17" s="2"/>
+      <c r="R17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK16">
+  <autoFilter ref="A1:AK17">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -2482,7 +2707,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI15">
+  <conditionalFormatting sqref="A2:AI16">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>